<commit_message>
fix: all bugs related to risk dashboard.
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_model_training\service_space\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC218B9-A309-4879-9E5B-EF3042602761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8598E37E-5DE9-4EDC-8CAD-674497C962CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>ASSET</t>
   </si>
@@ -48,16 +48,16 @@
     <t>INTERVAL</t>
   </si>
   <si>
-    <t>1d</t>
+    <t>Binance</t>
   </si>
   <si>
-    <t>Macro</t>
+    <t>ETH-USD</t>
   </si>
   <si>
-    <t>AV</t>
+    <t>Indicators</t>
   </si>
   <si>
-    <t>JPY=X</t>
+    <t>1d</t>
   </si>
 </sst>
 </file>
@@ -486,23 +486,23 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A4" sqref="A4:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="9" width="8.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="13" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="9" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="13" width="8.7109375" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="26" width="8.6640625" customWidth="1"/>
+    <col min="15" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.4">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,26 +538,26 @@
       <c r="T1" s="6"/>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>10</v>
+      <c r="A2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="6"/>
@@ -573,11 +573,11 @@
       <c r="T2" s="6"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
+      <c r="A3" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>150</v>
@@ -586,13 +586,13 @@
         <v>10</v>
       </c>
       <c r="E3" s="1">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="6"/>
@@ -608,27 +608,13 @@
       <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>200</v>
-      </c>
-      <c r="D4" s="1">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1">
-        <v>150</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2"/>
       <c r="I4" s="5"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -643,27 +629,13 @@
       <c r="T4" s="6"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
-        <v>250</v>
-      </c>
-      <c r="D5" s="1">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1">
-        <v>150</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
       <c r="I5" s="5"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
@@ -678,27 +650,13 @@
       <c r="T5" s="8"/>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1">
-        <v>300</v>
-      </c>
-      <c r="D6" s="1">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1">
-        <v>150</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="2"/>
       <c r="I6" s="5"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -716,27 +674,13 @@
       <c r="W6" s="8"/>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1">
-        <v>350</v>
-      </c>
-      <c r="D7" s="1">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1">
-        <v>150</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2"/>
       <c r="I7" s="5"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>

</xml_diff>

<commit_message>
feat: added custom factor feature, plus simple UI
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8598E37E-5DE9-4EDC-8CAD-674497C962CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B156D875-382B-4383-A8AD-7072750CC688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ASSET</t>
   </si>
@@ -54,7 +54,7 @@
     <t>ETH-USD</t>
   </si>
   <si>
-    <t>Indicators</t>
+    <t>Custom</t>
   </si>
   <si>
     <t>1d</t>
@@ -486,7 +486,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -551,7 +551,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="1">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
@@ -573,27 +573,13 @@
       <c r="T2" s="6"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1">
-        <v>150</v>
-      </c>
-      <c r="D3" s="1">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1">
-        <v>300</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2"/>
       <c r="I3" s="5"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>

</xml_diff>

<commit_message>
refactor: bug fixing. add: crypto_sentiment indicator.
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B156D875-382B-4383-A8AD-7072750CC688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D092D85-A4CA-4C44-A12B-95625AFD3B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,23 +486,23 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="13" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="5" width="10.5546875" customWidth="1"/>
+    <col min="6" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="13" width="8.6640625" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="26" width="8.7109375" customWidth="1"/>
+    <col min="15" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +551,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
add second version of target orientation
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC91D65F-1094-4C4D-80A3-A40F48C09638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED49DA5-93FF-472A-891E-15CDC21D7FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
add third version of target orientation
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED49DA5-93FF-472A-891E-15CDC21D7FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1377B0F-C669-4539-B969-F504A739AA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1512" yWindow="1032" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -215,9 +215,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:colOff>148590</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -486,7 +486,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Add benchmark to data preparation. Minor changes
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1377B0F-C669-4539-B969-F504A739AA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E68D5D-060A-4E90-B4E7-0A3A28A66AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1512" yWindow="1032" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="2640" windowWidth="21630" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Add data plots in tkinter UI
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6CE01D-31EE-4C19-8984-B4EFC75DE901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA15B69-EA7A-41CE-BB50-2F645562331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21060" yWindow="1956" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,13 @@
     <t>1d</t>
   </si>
   <si>
-    <t>NAVI</t>
+    <t>Custom</t>
   </si>
   <si>
-    <t>Yahoo</t>
+    <t>ETH-USD</t>
   </si>
   <si>
-    <t>Custom</t>
+    <t>Binance</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -530,10 +530,10 @@
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>150</v>
@@ -545,7 +545,7 @@
         <v>300</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
- Optimise dash app - Fix average line calcs - Fix add_predictions line
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA15B69-EA7A-41CE-BB50-2F645562331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFF7FC0-B75B-4F93-B549-20C443103D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21060" yWindow="1956" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="11">
   <si>
     <t>ASSET</t>
   </si>
@@ -48,16 +48,16 @@
     <t>INTERVAL</t>
   </si>
   <si>
-    <t>1d</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
     <t>ETH-USD</t>
   </si>
   <si>
     <t>Binance</t>
+  </si>
+  <si>
+    <t>Indicators</t>
+  </si>
+  <si>
+    <t>1h</t>
   </si>
 </sst>
 </file>
@@ -149,7 +149,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -530,25 +530,25 @@
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="1">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
-        <v>150</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="G2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>300</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>
@@ -564,13 +564,27 @@
       <c r="T2" s="5"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -585,13 +599,27 @@
       <c r="T3" s="5"/>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>60</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -606,13 +634,27 @@
       <c r="T4" s="5"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I5" s="4"/>
       <c r="J5" s="6"/>
       <c r="K5" s="7"/>
@@ -627,13 +669,27 @@
       <c r="T5" s="7"/>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>60</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -651,13 +707,27 @@
       <c r="W6" s="7"/>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>100</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -675,13 +745,27 @@
       <c r="W7" s="7"/>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1">
+        <v>100</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -699,34 +783,80 @@
       <c r="W8" s="7"/>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>60</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>100</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1">
+        <v>100</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -735,6 +865,7 @@
     </row>
     <row r="13" spans="1:23" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -743,6 +874,7 @@
     </row>
     <row r="14" spans="1:23" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -751,6 +883,7 @@
     </row>
     <row r="15" spans="1:23" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>

</xml_diff>

<commit_message>
Add SQLite module for saving directional accuracy score. Add timestamp as input for lstm research.
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFF7FC0-B75B-4F93-B549-20C443103D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC36465-2F27-4B92-82F3-13D7DEB2B4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ASSET</t>
   </si>
@@ -54,10 +54,10 @@
     <t>Binance</t>
   </si>
   <si>
-    <t>Indicators</t>
+    <t>1h</t>
   </si>
   <si>
-    <t>1h</t>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
@@ -262,7 +262,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:G15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:G31">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ASSET"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TYPE"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G12" sqref="A3:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -533,7 +533,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>60</v>
@@ -548,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>
@@ -564,27 +564,13 @@
       <c r="T2" s="5"/>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1">
-        <v>60</v>
-      </c>
-      <c r="D3" s="1">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1">
-        <v>100</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2"/>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -599,27 +585,13 @@
       <c r="T3" s="5"/>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <v>60</v>
-      </c>
-      <c r="D4" s="1">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1">
-        <v>100</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2"/>
       <c r="I4" s="4"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -634,27 +606,13 @@
       <c r="T4" s="5"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>60</v>
-      </c>
-      <c r="D5" s="1">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1">
-        <v>100</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
       <c r="I5" s="4"/>
       <c r="J5" s="6"/>
       <c r="K5" s="7"/>
@@ -669,27 +627,13 @@
       <c r="T5" s="7"/>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>60</v>
-      </c>
-      <c r="D6" s="1">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1">
-        <v>100</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="2"/>
       <c r="I6" s="4"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -707,27 +651,13 @@
       <c r="W6" s="7"/>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1">
-        <v>60</v>
-      </c>
-      <c r="D7" s="1">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1">
-        <v>100</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2"/>
       <c r="I7" s="4"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -745,27 +675,13 @@
       <c r="W7" s="7"/>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1">
-        <v>60</v>
-      </c>
-      <c r="D8" s="1">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1">
-        <v>100</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="2"/>
       <c r="I8" s="4"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -783,75 +699,33 @@
       <c r="W8" s="7"/>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1">
-        <v>60</v>
-      </c>
-      <c r="D9" s="1">
-        <v>6</v>
-      </c>
-      <c r="E9" s="1">
-        <v>100</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="2"/>
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>60</v>
-      </c>
-      <c r="D10" s="1">
-        <v>6</v>
-      </c>
-      <c r="E10" s="1">
-        <v>100</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="2"/>
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1">
-        <v>60</v>
-      </c>
-      <c r="D11" s="1">
-        <v>6</v>
-      </c>
-      <c r="E11" s="1">
-        <v>100</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="2"/>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1">
@@ -890,23 +764,151 @@
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:23" ht="15.75" customHeight="1">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add anomalies_detection module. Fix error with plotting run command 1\2 results.
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC36465-2F27-4B92-82F3-13D7DEB2B4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0827043-3808-46EA-867E-E507434CCC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,10 +54,10 @@
     <t>Binance</t>
   </si>
   <si>
-    <t>1h</t>
+    <t>Custom</t>
   </si>
   <si>
-    <t>Custom</t>
+    <t>1h</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="A3:G12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -533,7 +533,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>60</v>
@@ -548,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>

</xml_diff>

<commit_message>
Fixed binance hourly downloader bug.
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F05540C-BEA5-4545-B49D-D754C5FB97B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD1254C-F09F-496F-8A27-D447B9E18317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <t>Custom</t>
   </si>
   <si>
-    <t>1d</t>
+    <t>1h</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -536,10 +536,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>100</v>

</xml_diff>

<commit_message>
Optimized data collection and dash display.
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD1254C-F09F-496F-8A27-D447B9E18317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A460D6A-7279-4302-94AE-0397E2BABBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,16 +48,16 @@
     <t>INTERVAL</t>
   </si>
   <si>
+    <t>Custom</t>
+  </si>
+  <si>
     <t>ETH-USD</t>
   </si>
   <si>
     <t>Binance</t>
   </si>
   <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>1h</t>
+    <t>15m</t>
   </si>
 </sst>
 </file>
@@ -530,13 +530,13 @@
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
@@ -545,7 +545,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Added toggle to switch several models modes
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A460D6A-7279-4302-94AE-0397E2BABBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D41381-B294-44F6-B12A-68EE10FFAB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22245" yWindow="3105" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <t>Binance</t>
   </si>
   <si>
-    <t>15m</t>
+    <t>1h</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -536,10 +536,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="1">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1">
         <v>100</v>

</xml_diff>

<commit_message>
Added aditional tech indicators
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D41381-B294-44F6-B12A-68EE10FFAB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A496908C-3449-432A-9C34-7971F6BC925C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22245" yWindow="3105" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>INTERVAL</t>
   </si>
   <si>
-    <t>Custom</t>
-  </si>
-  <si>
     <t>ETH-USD</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>1h</t>
+  </si>
+  <si>
+    <t>Indicators</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -530,25 +530,25 @@
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>200</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1">
-        <v>100</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>

</xml_diff>

<commit_message>
Added sound effect for run_command_4.py
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A496908C-3449-432A-9C34-7971F6BC925C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EE5CF9-3D82-4305-8F0F-09137042A0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,16 +48,16 @@
     <t>INTERVAL</t>
   </si>
   <si>
-    <t>ETH-USD</t>
+    <t>Custom</t>
   </si>
   <si>
-    <t>Binance</t>
+    <t>1d</t>
   </si>
   <si>
-    <t>1h</t>
+    <t>EURJPY=X</t>
   </si>
   <si>
-    <t>Indicators</t>
+    <t>AV</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -530,25 +530,25 @@
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="1">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1">
-        <v>100</v>
-      </c>
-      <c r="D2" s="1">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>200</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>

</xml_diff>

<commit_message>
Add run_command_8.py to load and store data into db
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84CFFDB-A5ED-4759-930B-D497E85CF5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BE07E0-BB44-4321-BE1D-82AE5E44F96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3435" yWindow="3210" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,13 @@
     <t>Custom</t>
   </si>
   <si>
-    <t>1d</t>
+    <t>1wk</t>
   </si>
   <si>
-    <t>B</t>
+    <t>ETH-USD</t>
   </si>
   <si>
-    <t>XRP-USD</t>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -530,7 +530,7 @@
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -545,7 +545,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Add run_command_10.py (Volume analysis)
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BE07E0-BB44-4321-BE1D-82AE5E44F96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E50642-EBC3-4692-8ACA-DB701F846601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="3210" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,13 @@
     <t>Custom</t>
   </si>
   <si>
-    <t>1wk</t>
-  </si>
-  <si>
     <t>ETH-USD</t>
   </si>
   <si>
-    <t>M</t>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -530,7 +530,7 @@
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -539,7 +539,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
         <v>100</v>
@@ -548,7 +548,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>

</xml_diff>

<commit_message>
Refactor data visialisation and research_phase_two.py
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275ECB5C-AC16-4C95-BA7D-8C0E29DC3500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DAE36B-9538-447F-869E-6DE7637AB3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25050" yWindow="3045" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -539,7 +539,7 @@
         <v>70</v>
       </c>
       <c r="D2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
         <v>250</v>

</xml_diff>

<commit_message>
Task list 1. 21.11.24
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105EAD82-2C3E-4AFE-A0F3-28B522B6BE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62697E6F-6F56-42D8-96BE-06A9A8B835CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -536,13 +536,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="1">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Task list 2. 21.11.24 Task list 1. 22.11.24
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62697E6F-6F56-42D8-96BE-06A9A8B835CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E63375-7DA0-4B9F-A441-D2D8B2A0A928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,13 @@
     <t>Custom</t>
   </si>
   <si>
-    <t>1d</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
     <t>XRP-USD</t>
+  </si>
+  <si>
+    <t>1d</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -530,7 +530,7 @@
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -545,10 +545,10 @@
         <v>100</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="5"/>

</xml_diff>

<commit_message>
Task list 3. 21.11.24
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E63375-7DA0-4B9F-A441-D2D8B2A0A928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9671825E-084A-4EB3-8313-1E4CF14A6FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <t>XRP-USD</t>
   </si>
   <si>
-    <t>1d</t>
+    <t>1h</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Task list 1. 26.12.24
</commit_message>
<xml_diff>
--- a/run_commands/inputs/init.xlsx
+++ b/run_commands/inputs/init.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilsbo\PycharmProjects\plutus_lstm\run_commands\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9671825E-084A-4EB3-8313-1E4CF14A6FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C74356-B73F-48BA-8A1F-AB3E15A9226E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:W984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>